<commit_message>
added E2Esearch and add item to cart
</commit_message>
<xml_diff>
--- a/BestBuy_Project/allData/MenuLinkValidation.xlsx
+++ b/BestBuy_Project/allData/MenuLinkValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BestBuy_Project\BestBuy_Project\allData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68896F59-67D4-4CBE-A0B4-A324758C1446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3893E-AF59-40D1-B52A-3CF4E107C3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6810" yWindow="3360" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="142">
   <si>
     <t>Top Deals</t>
   </si>
@@ -781,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3B181F-31C9-4C4D-B96E-53B0DF133C1B}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,156 +817,24 @@
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="1" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>